<commit_message>
minor fix to notes column
</commit_message>
<xml_diff>
--- a/aeroponics spreadsheet.xlsx
+++ b/aeroponics spreadsheet.xlsx
@@ -160,7 +160,7 @@
     <t>foam inserts</t>
   </si>
   <si>
-    <t>ongoing cost per plant</t>
+    <t>ongoing cost per spin per section</t>
   </si>
   <si>
     <t>total per section</t>
@@ -274,7 +274,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:I26"/>
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>